<commit_message>
Some more woring slides - starting to look ok
</commit_message>
<xml_diff>
--- a/Phantomresults/data.xlsx
+++ b/Phantomresults/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\Documents\Undervisning\NSNMSiemens\Phantomresults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B15B4F4-C81E-47ED-9104-A91821FDE4BD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D32AE1-B695-4EE2-9B76-E2A91AAB75DF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="11910" xr2:uid="{8B869A33-6C3B-49D1-9D01-0D858346E3E3}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="11910" xr2:uid="{8B869A33-6C3B-49D1-9D01-0D858346E3E3}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -394,10 +394,13 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="21" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -685,7 +688,7 @@
         <v>3.1524044252828551E-2</v>
       </c>
       <c r="E17">
-        <v>6.3048088505657102E-2</v>
+        <v>6.5480507612352495E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -702,7 +705,7 @@
         <v>3.1524044252828551E-2</v>
       </c>
       <c r="E18">
-        <v>0.1260961770113142</v>
+        <v>0.1260997997464052</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -719,7 +722,7 @@
         <v>3.1524044252828551E-2</v>
       </c>
       <c r="E19">
-        <v>0.25219235402262841</v>
+        <v>0.25816899703943336</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -736,7 +739,7 @@
         <v>3.1524044252828551E-2</v>
       </c>
       <c r="E20">
-        <v>0.50438470804525681</v>
+        <v>0.50301086914733539</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -753,7 +756,7 @@
         <v>3.1524044252828551E-2</v>
       </c>
       <c r="E21">
-        <v>3.5622170005696261</v>
+        <v>3.4604660149691666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>